<commit_message>
Added minor results for MasterDiplom
</commit_message>
<xml_diff>
--- a/Dens_matrix_qubit/Results.xlsx
+++ b/Dens_matrix_qubit/Results.xlsx
@@ -808,27 +808,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>0.5584042537597934</t>
+          <t>0.5559839614875356</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>0.9618230942606429</t>
+          <t>0.9276750430740468</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>0.9975921671080856</t>
+          <t>0.9935404298917957</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>0.9998388444234491</t>
+          <t>0.9995915976099383</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>0.999998875883651</t>
+          <t>0.9999996732049408</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -845,27 +845,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0.5127998570406993</t>
+          <t>0.5158054877847658</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.9316886065887571</t>
+          <t>0.9569204571328191</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.9946250802076204</t>
+          <t>0.9949509219699387</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.9997837727805233</t>
+          <t>0.9997494041500106</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.9999983233423682</t>
+          <t>0.9999998705981143</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -882,27 +882,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>0.5051582853981411</t>
+          <t>0.5066973956625889</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.938060849270967</t>
+          <t>0.9517112925674315</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.9930413477657452</t>
+          <t>0.9953900700852497</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.9997516786304232</t>
+          <t>0.9997887990788891</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.9999981685046463</t>
+          <t>0.9999998484275074</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -919,27 +919,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>0.5054664764164286</t>
+          <t>0.5043441205810106</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.9297675717422639</t>
+          <t>0.949951866238407</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9897028744537435</t>
+          <t>0.9951855792042685</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.9990531027882543</t>
+          <t>0.9998324788456466</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.9999890275822683</t>
+          <t>0.9999999292953776</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -956,27 +956,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>0.5019529830444874</t>
+          <t>0.5046621137639407</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0.9329113213605383</t>
+          <t>0.9509282401531843</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9900399724572762</t>
+          <t>0.9946905471162312</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.998784073138979</t>
+          <t>0.9998283016044427</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.9999819792194811</t>
+          <t>0.9999999443158842</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -993,27 +993,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>0.5021976733104386</t>
+          <t>0.5028753796909075</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0.9274442098724462</t>
+          <t>0.9521548411290554</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.9869844348288133</t>
+          <t>0.9949823254973134</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.9985609141833474</t>
+          <t>0.9998189019473729</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.9999391779245901</t>
+          <t>0.9999999469827321</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1030,27 +1030,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>0.5047969607042211</t>
+          <t>0.5017464050989884</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0.9368259739858148</t>
+          <t>0.9518237955844949</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.9885268081171439</t>
+          <t>0.9948808300856948</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.9986096149840189</t>
+          <t>0.9998311666357742</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.9999209083837068</t>
+          <t>0.999999934526085</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1067,27 +1067,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>0.5073740776338163</t>
+          <t>0.5061910602324473</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0.928598533748687</t>
+          <t>0.9512385494882523</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.9890517865106702</t>
+          <t>0.9952109328298336</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.9983538457990512</t>
+          <t>0.9998052694530802</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.9998735424505105</t>
+          <t>0.9999999035841519</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1104,27 +1104,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>0.5133483826368926</t>
+          <t>0.5112106602408916</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>0.941931566092905</t>
+          <t>0.9559861689750272</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.9880912493911552</t>
+          <t>0.9949761371894336</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.9982700903827777</t>
+          <t>0.9997627551198304</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.9998739507930946</t>
+          <t>0.9999998671778866</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1141,27 +1141,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>0.5492118316102637</t>
+          <t>0.545148932189429</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0.9002437580408467</t>
+          <t>0.9311619612766192</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.9844714083144935</t>
+          <t>0.9938775975353399</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.9974087990498285</t>
+          <t>0.9995894712881097</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.9998266273514499</t>
+          <t>0.9999996066470124</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">

</xml_diff>